<commit_message>
converter release! file saving
</commit_message>
<xml_diff>
--- a/converter/src/test/resources/conversions_from.xlsx
+++ b/converter/src/test/resources/conversions_from.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\kotlin\AlfaConverter\converter\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C1969B-EFA1-40BF-A303-8AB845247F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C61683-4AAC-4ABD-B652-0CAEA0CD3648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20550" yWindow="2595" windowWidth="15525" windowHeight="10965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24465" yWindow="2745" windowWidth="15525" windowHeight="10965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
   <si>
     <t>Column to bind 1</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>merged</t>
+  </si>
+  <si>
+    <t>who?</t>
+  </si>
+  <si>
+    <t>me</t>
   </si>
 </sst>
 </file>
@@ -369,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -381,7 +387,7 @@
     <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -400,8 +406,11 @@
       <c r="F1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -420,8 +429,11 @@
       <c r="F2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20</v>
       </c>
@@ -440,8 +452,11 @@
       <c r="F3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>30</v>
       </c>
@@ -460,8 +475,11 @@
       <c r="F4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>40</v>
       </c>
@@ -480,8 +498,11 @@
       <c r="F5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>50</v>
       </c>
@@ -500,8 +521,11 @@
       <c r="F6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>60</v>
       </c>
@@ -520,8 +544,11 @@
       <c r="F7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>70</v>
       </c>
@@ -540,8 +567,11 @@
       <c r="F8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>80</v>
       </c>
@@ -560,8 +590,11 @@
       <c r="F9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>90</v>
       </c>
@@ -579,6 +612,9 @@
       </c>
       <c r="F10">
         <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>